<commit_message>
update the workflow based on Euan's comments, including: add black list add new donors and agencies and channels add new keywords add markers for projects that are not fully climate
</commit_message>
<xml_diff>
--- a/Data/auxiliary/Climate filters.xlsx
+++ b/Data/auxiliary/Climate filters.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yutian/Dropbox/PARIS21/R/PRESS/Data/auxiliary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47DD6EC7-8FD0-9F4F-8045-A5332EB2EE59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB01987D-7E23-3242-B493-693DAA5788E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{09E330C0-9EC0-F649-A29C-8A61868745D7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{09E330C0-9EC0-F649-A29C-8A61868745D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Agency" sheetId="1" r:id="rId1"/>
     <sheet name="Donor" sheetId="2" r:id="rId2"/>
     <sheet name="Channel codes" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Agency!$A$1:$J$732</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Channel codes'!$A$1:$Q$405</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7084" uniqueCount="2756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7089" uniqueCount="2756">
   <si>
     <t>donorcode</t>
   </si>
@@ -8552,7 +8556,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -8714,6 +8718,21 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -9034,8 +9053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50187964-6686-114D-83B9-CC244A431179}">
   <dimension ref="A1:J798"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="182" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -25240,7 +25259,9 @@
       <c r="E547" s="2" t="s">
         <v>1070</v>
       </c>
-      <c r="F547" s="2"/>
+      <c r="F547" s="2">
+        <v>2</v>
+      </c>
       <c r="G547" s="2" t="s">
         <v>1071</v>
       </c>
@@ -25270,7 +25291,9 @@
       <c r="E548" s="2" t="s">
         <v>1073</v>
       </c>
-      <c r="F548" s="2"/>
+      <c r="F548" s="2">
+        <v>2</v>
+      </c>
       <c r="G548" s="2" t="s">
         <v>1074</v>
       </c>
@@ -25298,7 +25321,9 @@
       <c r="E549" s="2" t="s">
         <v>1075</v>
       </c>
-      <c r="F549" s="2"/>
+      <c r="F549" s="2">
+        <v>2</v>
+      </c>
       <c r="G549" s="2" t="s">
         <v>1076</v>
       </c>
@@ -25360,7 +25385,9 @@
       <c r="E551" s="2" t="s">
         <v>1081</v>
       </c>
-      <c r="F551" s="2"/>
+      <c r="F551" s="2">
+        <v>2</v>
+      </c>
       <c r="G551" s="2" t="s">
         <v>1082</v>
       </c>
@@ -25390,7 +25417,9 @@
       <c r="E552" s="2" t="s">
         <v>1084</v>
       </c>
-      <c r="F552" s="2"/>
+      <c r="F552" s="2">
+        <v>2</v>
+      </c>
       <c r="G552" s="2" t="s">
         <v>1085</v>
       </c>
@@ -25420,7 +25449,9 @@
       <c r="E553" s="2" t="s">
         <v>1087</v>
       </c>
-      <c r="F553" s="2"/>
+      <c r="F553" s="2">
+        <v>2</v>
+      </c>
       <c r="G553" s="2" t="s">
         <v>1088</v>
       </c>
@@ -28586,7 +28617,9 @@
       <c r="E659" s="2" t="s">
         <v>1331</v>
       </c>
-      <c r="F659" s="2"/>
+      <c r="F659" s="2">
+        <v>1</v>
+      </c>
       <c r="G659" s="2" t="s">
         <v>1331</v>
       </c>
@@ -28616,7 +28649,9 @@
       <c r="E660" s="2" t="s">
         <v>1332</v>
       </c>
-      <c r="F660" s="2"/>
+      <c r="F660" s="2">
+        <v>1</v>
+      </c>
       <c r="G660" s="2" t="s">
         <v>1332</v>
       </c>
@@ -28676,7 +28711,9 @@
       <c r="E662" s="2" t="s">
         <v>1335</v>
       </c>
-      <c r="F662" s="2"/>
+      <c r="F662" s="2">
+        <v>2</v>
+      </c>
       <c r="G662" s="2" t="s">
         <v>1336</v>
       </c>
@@ -29150,7 +29187,9 @@
       <c r="E678" s="2" t="s">
         <v>1381</v>
       </c>
-      <c r="F678" s="2"/>
+      <c r="F678" s="2">
+        <v>2</v>
+      </c>
       <c r="G678" s="2" t="s">
         <v>1381</v>
       </c>
@@ -29180,7 +29219,9 @@
       <c r="E679" s="2" t="s">
         <v>1383</v>
       </c>
-      <c r="F679" s="2"/>
+      <c r="F679" s="2">
+        <v>2</v>
+      </c>
       <c r="G679" s="2" t="s">
         <v>1383</v>
       </c>
@@ -29210,7 +29251,9 @@
       <c r="E680" s="2" t="s">
         <v>1385</v>
       </c>
-      <c r="F680" s="2"/>
+      <c r="F680" s="2">
+        <v>2</v>
+      </c>
       <c r="G680" s="2" t="s">
         <v>1385</v>
       </c>
@@ -29240,7 +29283,9 @@
       <c r="E681" s="2" t="s">
         <v>1387</v>
       </c>
-      <c r="F681" s="2"/>
+      <c r="F681" s="2">
+        <v>2</v>
+      </c>
       <c r="G681" s="2" t="s">
         <v>1387</v>
       </c>
@@ -31485,21 +31530,22 @@
       <c r="J798" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J732" xr:uid="{50187964-6686-114D-83B9-CC244A431179}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40461A02-8CC5-374F-A5DF-469BB5A95F37}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>1488</v>
       </c>
@@ -31509,8 +31555,11 @@
       <c r="C1" s="5" t="s">
         <v>1490</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1011</v>
       </c>
@@ -31520,8 +31569,11 @@
       <c r="C2" s="6" t="s">
         <v>1297</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>1016</v>
       </c>
@@ -31530,6 +31582,37 @@
       </c>
       <c r="C3" s="6" t="s">
         <v>1330</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="62">
+        <v>1313</v>
+      </c>
+      <c r="B4" s="62" t="s">
+        <v>1379</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>1380</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="62">
+        <v>811</v>
+      </c>
+      <c r="B5" s="62" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -31541,11 +31624,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A601A20-81E1-804C-80F8-920075A12FA8}">
   <dimension ref="A1:Q405"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView zoomScale="137" workbookViewId="0">
+      <selection activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="24.6640625" style="61" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
@@ -31600,7 +31686,7 @@
         <v>1506</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="17" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" s="17" customFormat="1" ht="48" x14ac:dyDescent="0.15">
       <c r="A2" s="12">
         <v>10000</v>
       </c>
@@ -32166,7 +32252,7 @@
       <c r="D19" s="20" t="s">
         <v>1543</v>
       </c>
-      <c r="E19" s="29" t="s">
+      <c r="E19" s="58" t="s">
         <v>1544</v>
       </c>
       <c r="F19" s="29"/>
@@ -34718,7 +34804,7 @@
         <v>2021</v>
       </c>
       <c r="D81" s="35"/>
-      <c r="E81" s="35" t="s">
+      <c r="E81" s="31" t="s">
         <v>1737</v>
       </c>
       <c r="F81" s="35"/>
@@ -35281,7 +35367,9 @@
       <c r="E95" s="20" t="s">
         <v>1335</v>
       </c>
-      <c r="F95" s="20"/>
+      <c r="F95" s="20">
+        <v>2</v>
+      </c>
       <c r="G95" s="20" t="s">
         <v>1337</v>
       </c>
@@ -35324,7 +35412,9 @@
       <c r="E96" s="38" t="s">
         <v>1785</v>
       </c>
-      <c r="F96" s="38"/>
+      <c r="F96" s="38">
+        <v>2</v>
+      </c>
       <c r="G96" s="38" t="s">
         <v>1784</v>
       </c>
@@ -35668,7 +35758,9 @@
       <c r="E104" s="20" t="s">
         <v>1812</v>
       </c>
-      <c r="F104" s="20"/>
+      <c r="F104" s="20">
+        <v>2</v>
+      </c>
       <c r="G104" s="20" t="s">
         <v>1811</v>
       </c>
@@ -36301,7 +36393,7 @@
       </c>
       <c r="C120" s="44"/>
       <c r="D120" s="45"/>
-      <c r="E120" s="46" t="s">
+      <c r="E120" s="47" t="s">
         <v>1863</v>
       </c>
       <c r="F120" s="46"/>
@@ -38043,7 +38135,7 @@
       </c>
       <c r="C160" s="44"/>
       <c r="D160" s="45"/>
-      <c r="E160" s="52" t="s">
+      <c r="E160" s="59" t="s">
         <v>2008</v>
       </c>
       <c r="F160" s="52"/>
@@ -38074,7 +38166,7 @@
       <c r="D161" s="20" t="s">
         <v>2010</v>
       </c>
-      <c r="E161" s="53" t="s">
+      <c r="E161" s="60" t="s">
         <v>2011</v>
       </c>
       <c r="F161" s="53"/>
@@ -38929,7 +39021,7 @@
       </c>
       <c r="C180" s="44"/>
       <c r="D180" s="45"/>
-      <c r="E180" s="46" t="s">
+      <c r="E180" s="47" t="s">
         <v>2090</v>
       </c>
       <c r="F180" s="46"/>
@@ -39091,7 +39183,7 @@
       <c r="D184" s="55" t="s">
         <v>2100</v>
       </c>
-      <c r="E184" s="55" t="s">
+      <c r="E184" s="20" t="s">
         <v>2101</v>
       </c>
       <c r="F184" s="55"/>
@@ -39249,7 +39341,7 @@
       </c>
       <c r="C188" s="44"/>
       <c r="D188" s="45"/>
-      <c r="E188" s="46" t="s">
+      <c r="E188" s="47" t="s">
         <v>2114</v>
       </c>
       <c r="F188" s="46"/>
@@ -43388,7 +43480,9 @@
       <c r="E286" s="20" t="s">
         <v>2441</v>
       </c>
-      <c r="F286" s="20"/>
+      <c r="F286" s="20">
+        <v>2</v>
+      </c>
       <c r="G286" s="20" t="s">
         <v>2442</v>
       </c>
@@ -43480,7 +43574,9 @@
       <c r="E288" s="20" t="s">
         <v>2448</v>
       </c>
-      <c r="F288" s="20"/>
+      <c r="F288" s="20">
+        <v>2</v>
+      </c>
       <c r="G288" s="20" t="s">
         <v>2449</v>
       </c>
@@ -43613,7 +43709,9 @@
       <c r="E291" s="20" t="s">
         <v>1379</v>
       </c>
-      <c r="F291" s="20"/>
+      <c r="F291" s="20">
+        <v>2</v>
+      </c>
       <c r="G291" s="20" t="s">
         <v>2456</v>
       </c>
@@ -44381,7 +44479,9 @@
       <c r="E309" s="20" t="s">
         <v>2510</v>
       </c>
-      <c r="F309" s="20"/>
+      <c r="F309" s="20">
+        <v>2</v>
+      </c>
       <c r="G309" s="20" t="s">
         <v>2509</v>
       </c>
@@ -48083,6 +48183,7 @@
       <c r="Q405" s="16"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Q405" xr:uid="{6A601A20-81E1-804C-80F8-920075A12FA8}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>